<commit_message>
add Seurat 3 script
</commit_message>
<xml_diff>
--- a/doc/singler.colors.xlsx
+++ b/doc/singler.colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yah2014/Dropbox/Public/Olivier/Projects/scRNAseq-MCL/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yah2014/Dropbox/Public/Olivier/Projects/scRNAseq-BladderCancer/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9BB2CF-D2D5-D244-A7B4-9270DF25553B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8EDE10-EB71-4346-938E-753AD5101E4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{FD2BDCDE-9325-2D42-91C9-863AAE358120}"/>
+    <workbookView xWindow="28800" yWindow="-6280" windowWidth="33600" windowHeight="16500" xr2:uid="{FD2BDCDE-9325-2D42-91C9-863AAE358120}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="156">
   <si>
     <t>#7FC97F</t>
   </si>
@@ -297,9 +297,6 @@
     <t>T_cell:gamma-delta</t>
   </si>
   <si>
-    <t>singler.color2</t>
-  </si>
-  <si>
     <t>CD4+ T-cells</t>
   </si>
   <si>
@@ -436,6 +433,66 @@
   </si>
   <si>
     <t>#4038b0</t>
+  </si>
+  <si>
+    <t>Adipocytes</t>
+  </si>
+  <si>
+    <t>B cells</t>
+  </si>
+  <si>
+    <t>Dendritic cells</t>
+  </si>
+  <si>
+    <t>Endothelial cells</t>
+  </si>
+  <si>
+    <t>Fibroblasts</t>
+  </si>
+  <si>
+    <t>Fibroblasts activated</t>
+  </si>
+  <si>
+    <t>Fibroblasts senescent</t>
+  </si>
+  <si>
+    <t>Granulocytes</t>
+  </si>
+  <si>
+    <t>Hepatocytes</t>
+  </si>
+  <si>
+    <t>Macrophages</t>
+  </si>
+  <si>
+    <t>Macrophages activated</t>
+  </si>
+  <si>
+    <t>NPCs</t>
+  </si>
+  <si>
+    <t>T cells</t>
+  </si>
+  <si>
+    <t>singler_F_BladderCancer_M3_20190606</t>
+  </si>
+  <si>
+    <t>#ff0000</t>
+  </si>
+  <si>
+    <t>#e94749</t>
+  </si>
+  <si>
+    <t>singler_F_BladderCancer_mm10_6_20190706</t>
+  </si>
+  <si>
+    <t>other cell types</t>
+  </si>
+  <si>
+    <t>Epithelial cells</t>
+  </si>
+  <si>
+    <t>Stromal cells</t>
   </si>
 </sst>
 </file>
@@ -1825,13 +1882,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1869,7 +1926,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1908,7 +1965,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1947,7 +2004,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1986,7 +2043,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2597,13 +2654,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>203200</xdr:rowOff>
@@ -2993,7 +3050,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -3032,7 +3089,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3071,7 +3128,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -3110,7 +3167,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -3149,7 +3206,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -3188,7 +3245,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
@@ -3227,7 +3284,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3266,7 +3323,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -3305,7 +3362,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3344,7 +3401,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3383,7 +3440,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4654,7 +4711,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4693,7 +4750,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4732,7 +4789,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4771,7 +4828,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4888,7 +4945,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4966,7 +5023,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5083,7 +5140,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -5122,7 +5179,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5161,7 +5218,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5200,7 +5257,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5239,7 +5296,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -5278,7 +5335,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5317,7 +5374,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5356,13 +5413,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5400,7 +5457,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5439,7 +5496,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5595,7 +5652,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5634,7 +5691,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5673,7 +5730,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5712,7 +5769,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -5751,7 +5808,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5790,7 +5847,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5829,7 +5886,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5868,7 +5925,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5907,7 +5964,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5946,7 +6003,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5985,7 +6042,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6024,7 +6081,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6063,7 +6120,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -6102,7 +6159,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6141,7 +6198,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6180,7 +6237,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6219,7 +6276,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6258,7 +6315,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6297,7 +6354,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6336,7 +6393,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6375,7 +6432,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6414,7 +6471,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6453,7 +6510,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6492,13 +6549,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>6604</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>201168</xdr:rowOff>
@@ -6536,7 +6593,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6575,7 +6632,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6614,7 +6671,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6653,13 +6710,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>6604</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>201168</xdr:rowOff>
@@ -6697,7 +6754,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6736,7 +6793,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6775,7 +6832,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6814,7 +6871,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6853,7 +6910,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6892,7 +6949,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6931,13 +6988,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>6604</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>201168</xdr:rowOff>
@@ -6975,7 +7032,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7014,7 +7071,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7042,6 +7099,1108 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4953000" y="1295400"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="159" name="Picture 158">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56C68139-4B55-D24F-932A-AAC9E8D1CEE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="215900"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="160" name="Picture 159">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AF79911-47E8-3C4E-9382-C963E44B4D90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="431800"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="162" name="Picture 161">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{717F4AA7-C7F9-EC4C-B93D-90761B55BC20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="1727200"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28448</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>201168</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="177" name="Picture 176">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBF3FC7D-5441-3349-BD63-556BBCFE0F1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId75"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4965700" y="3454400"/>
+          <a:ext cx="841248" cy="201168"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="186" name="Picture 185">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AD3EAC5-3227-5B43-BE14-8C7B67D506A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10109200" y="7531100"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="189" name="Picture 188">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CAAE5E6-BDCE-B242-89F6-36E8F88462A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10109200" y="3886200"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="197" name="Picture 196">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC1A776-99AC-3C4B-B90A-FAB2ED077811}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId69"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10109200" y="4965700"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="208" name="Picture 207">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87E0D85A-E90E-C845-B409-036119E54B6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="4749800"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="210" name="Picture 209">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DCD9E3E-86F8-4F43-829C-61332010DF00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="863600"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="212" name="Picture 211">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D603C05-21EE-EE49-A9AF-D80486159113}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1651000" y="2806700"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="841248" cy="201168"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="213" name="Picture 212">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{887E32A8-4D11-D941-AC3D-612FD45846E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId76"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="3022600"/>
+          <a:ext cx="841248" cy="201168"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="227" name="Picture 226">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4924E94D-4AB0-4043-8DEB-D1D6C533E256}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="3238500"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="228" name="Picture 227">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5205189F-BEB3-8543-BBE6-7FB2CB26028A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="4102100"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="229" name="Picture 228">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45DC0BF-179D-4346-B1C3-29C6F0DFA929}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId67"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10109200" y="5181600"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="832104" cy="201168"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="234" name="Picture 233">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B33E6A7-57F5-E84E-BAB1-7C4E088B1758}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId73"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10109200" y="3022600"/>
+          <a:ext cx="832104" cy="201168"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="239" name="Picture 238">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E226726-375D-7B46-A064-F2865A91CB67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1651000" y="3022600"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="192" name="Picture 191">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E6B3C9F-8817-F44F-8530-C8D27677C0EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8255000" y="431800"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="253" name="Picture 252">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CFEE333-3C45-1D48-B322-68A77C1AA8A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8255000" y="863600"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="190" name="Picture 189">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEC2B986-6541-8B48-A1A6-B68FEE3D38FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1663700" y="4533900"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="240" name="Picture 239">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5527EC55-D4ED-1E44-88DB-67ECC83EB4B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4127500" y="2590800"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="267" name="Picture 266">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F92144A-03B1-094D-95BB-189C4984244A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9283700" y="3022600"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="270" name="Picture 269">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03428F25-05AB-EB4B-A032-BED12D3D3382}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4127500" y="3238500"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="272" name="Picture 271">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9426322B-8B4B-3147-8D03-69440D5E0EEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="2806700"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="275" name="Picture 274">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7598DF48-8EF3-1E46-A141-BDFC20E46FE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1663700" y="3238500"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="276" name="Picture 275">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{251212D4-83B9-AC4B-80A6-E1B54267D7D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1663700" y="660400"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="198" name="Picture 197">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4DF30CB-4CA7-4440-806F-AD385D2B0450}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId69"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9283700" y="1727200"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="206" name="Picture 205">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458C9DD1-E8F3-A34A-9A1E-C5D7AF32C644}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15265400" y="3238500"/>
+          <a:ext cx="838200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838200" cy="203200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="242" name="Picture 241">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{170FADDA-43BA-E443-90DB-F64BFAA9F790}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="3886200"/>
           <a:ext cx="838200" cy="203200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7351,51 +8510,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F425B8D6-F52F-D847-96BE-ADA617D7BA82}">
-  <dimension ref="A1:P91"/>
+  <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="50" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="50" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50" customWidth="1"/>
+    <col min="20" max="20" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>73</v>
       </c>
       <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" t="s">
         <v>74</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="H1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" t="s">
-        <v>90</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>133</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7405,26 +8575,44 @@
       <c r="D2" t="s">
         <v>71</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="3">
+        <v>705</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" s="3">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="R2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T2" s="3">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="U2" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7434,26 +8622,44 @@
       <c r="D3" t="s">
         <v>71</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2619</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="M3" s="3">
+        <v>120</v>
+      </c>
+      <c r="P3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="J3" s="3">
+      <c r="R3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="T3" s="3">
         <v>4</v>
       </c>
-      <c r="K3" t="s">
+      <c r="U3" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7463,30 +8669,48 @@
       <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1258</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="M4" s="3">
+        <v>96</v>
+      </c>
+      <c r="P4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J4" s="3">
+      <c r="R4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="T4" s="3">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
+      <c r="V4" t="s">
         <v>63</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="O4" s="3">
+      <c r="X4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y4" s="3">
         <v>1298</v>
       </c>
-      <c r="P4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7496,30 +8720,48 @@
       <c r="D5" t="s">
         <v>71</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2355</v>
+      </c>
+      <c r="J5" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="L5" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M5" s="3">
+        <v>596</v>
+      </c>
+      <c r="P5" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T5" s="3">
         <v>5236</v>
       </c>
-      <c r="L5" t="s">
+      <c r="V5" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="O5" s="3">
+      <c r="X5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y5" s="3">
         <v>1014</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7529,30 +8771,48 @@
       <c r="D6" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="3">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>150</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" s="3">
+        <v>7</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="J6" s="3">
+      <c r="R6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="T6" s="3">
         <v>2696</v>
       </c>
-      <c r="L6" t="s">
+      <c r="V6" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="O6" s="3">
+      <c r="X6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y6" s="3">
         <v>473</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7562,30 +8822,48 @@
       <c r="D7" t="s">
         <v>71</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="3">
+        <v>251</v>
+      </c>
+      <c r="J7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M7" s="3">
+        <v>50</v>
+      </c>
+      <c r="P7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="J7" s="3">
+      <c r="R7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="T7" s="3">
         <v>7743</v>
       </c>
-      <c r="L7" t="s">
+      <c r="V7" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="O7" s="3">
+      <c r="X7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y7" s="3">
         <v>1029</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7595,30 +8873,48 @@
       <c r="D8" t="s">
         <v>71</v>
       </c>
-      <c r="F8" t="s">
-        <v>134</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="J8" s="3">
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2464</v>
+      </c>
+      <c r="J8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1578</v>
+      </c>
+      <c r="P8" t="s">
+        <v>133</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="T8" s="3">
         <v>24</v>
       </c>
-      <c r="L8" t="s">
+      <c r="V8" t="s">
         <v>48</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="O8" s="3">
+      <c r="X8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y8" s="3">
         <v>608</v>
       </c>
-      <c r="P8" s="3"/>
+      <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7628,24 +8924,42 @@
       <c r="D9" t="s">
         <v>71</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3072</v>
+      </c>
+      <c r="J9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="M9" s="3">
+        <v>4877</v>
+      </c>
+      <c r="P9" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="J9" s="3">
+      <c r="R9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="T9" s="3">
         <v>33</v>
       </c>
-      <c r="K9" t="s">
+      <c r="U9" t="s">
         <v>62</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7655,30 +8969,48 @@
       <c r="D10" t="s">
         <v>69</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="3">
+        <v>340</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="M10" s="3">
+        <v>210</v>
+      </c>
+      <c r="P10" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J10" s="3">
+      <c r="R10" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="T10" s="3">
         <v>2</v>
       </c>
-      <c r="L10" t="s">
+      <c r="V10" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="O10" s="3">
+      <c r="X10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y10" s="3">
         <v>553</v>
       </c>
-      <c r="P10" s="3"/>
+      <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7689,20 +9021,38 @@
         <v>71</v>
       </c>
       <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="3">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1231</v>
+      </c>
+      <c r="O11" t="s">
         <v>30</v>
       </c>
-      <c r="L11" t="s">
-        <v>136</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="O11" s="3">
+      <c r="V11" t="s">
+        <v>135</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y11" s="3">
         <v>17</v>
       </c>
-      <c r="P11" s="3"/>
+      <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -7713,20 +9063,38 @@
         <v>69</v>
       </c>
       <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="3">
+        <v>10592</v>
+      </c>
+      <c r="J12" t="s">
+        <v>151</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M12" s="3">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
         <v>31</v>
       </c>
-      <c r="L12" t="s">
+      <c r="V12" t="s">
         <v>42</v>
       </c>
-      <c r="N12" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="O12" s="3">
+      <c r="X12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y12" s="3">
         <v>2</v>
       </c>
-      <c r="P12" s="3"/>
+      <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -7737,21 +9105,39 @@
         <v>71</v>
       </c>
       <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="3">
+        <v>753</v>
+      </c>
+      <c r="J13" t="s">
+        <v>134</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M13" s="3">
+        <v>102</v>
+      </c>
+      <c r="O13" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="L13" t="s">
+      <c r="R13" s="3"/>
+      <c r="V13" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="O13" s="3">
+      <c r="X13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y13" s="3">
         <v>2</v>
       </c>
-      <c r="P13" s="3"/>
+      <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -7761,22 +9147,33 @@
       <c r="D14" t="s">
         <v>71</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="J14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" s="3">
+        <v>484</v>
+      </c>
+      <c r="O14" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="L14" t="s">
-        <v>135</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="O14" s="3">
+      <c r="R14" s="3"/>
+      <c r="V14" t="s">
+        <v>134</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y14" s="3">
         <v>101</v>
       </c>
-      <c r="P14" s="3"/>
+      <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -7786,31 +9183,42 @@
       <c r="D15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" t="s">
-        <v>135</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J15" s="3">
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="J15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M15" s="3">
+        <v>35</v>
+      </c>
+      <c r="O15" s="3"/>
+      <c r="P15" t="s">
+        <v>134</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="T15" s="3">
         <v>80</v>
       </c>
-      <c r="L15" t="s">
+      <c r="V15" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="X15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="O15" s="3">
+      <c r="Y15" s="3">
         <v>18</v>
       </c>
-      <c r="P15" s="3"/>
+      <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -7820,31 +9228,42 @@
       <c r="D16" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" t="s">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="J16" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="M16" s="3">
+        <v>8</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="R16" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="S16" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="3">
+      <c r="T16" s="3">
         <v>14</v>
       </c>
-      <c r="L16" t="s">
+      <c r="V16" t="s">
         <v>21</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="O16" s="3">
+      <c r="X16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y16" s="3">
         <v>6</v>
       </c>
-      <c r="P16" s="3"/>
+      <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -7854,16 +9273,27 @@
       <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="M17" s="3">
+        <v>247</v>
+      </c>
+      <c r="O17" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="K17" t="s">
+      <c r="R17" s="3"/>
+      <c r="U17" t="s">
         <v>23</v>
       </c>
-      <c r="P17" s="3"/>
+      <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -7873,31 +9303,33 @@
       <c r="D18" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" t="s">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="R18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="S18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J18" s="3">
+      <c r="T18" s="3">
         <v>1</v>
       </c>
-      <c r="L18" t="s">
+      <c r="V18" t="s">
         <v>60</v>
       </c>
-      <c r="N18" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="O18" s="3">
+      <c r="X18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y18" s="3">
         <v>11</v>
       </c>
-      <c r="P18" s="3"/>
+      <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -7907,31 +9339,31 @@
       <c r="D19" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" t="s">
+      <c r="O19" s="3"/>
+      <c r="P19" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J19" s="3">
+      <c r="R19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="T19" s="3">
         <v>38</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="V19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="O19" s="3">
+      <c r="X19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y19" s="3">
         <v>11961</v>
       </c>
-      <c r="P19" s="3"/>
+      <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -7941,31 +9373,31 @@
       <c r="D20" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" t="s">
+      <c r="O20" s="3"/>
+      <c r="P20" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J20" s="3">
+      <c r="R20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="T20" s="3">
         <v>9</v>
       </c>
-      <c r="L20" t="s">
+      <c r="V20" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O20" s="3">
+      <c r="X20" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y20" s="3">
         <v>32</v>
       </c>
-      <c r="P20" s="3"/>
+      <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -7975,31 +9407,31 @@
       <c r="D21" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" t="s">
+      <c r="O21" s="3"/>
+      <c r="P21" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="J21" s="3">
+      <c r="R21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="T21" s="3">
         <v>8</v>
       </c>
-      <c r="L21" t="s">
+      <c r="V21" t="s">
         <v>18</v>
       </c>
-      <c r="N21" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="O21" s="3">
+      <c r="X21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y21" s="3">
         <v>1524</v>
       </c>
-      <c r="P21" s="3"/>
+      <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8009,31 +9441,31 @@
       <c r="D22" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" t="s">
+      <c r="O22" s="3"/>
+      <c r="P22" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="R22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="S22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J22" s="3">
+      <c r="T22" s="3">
         <v>1008</v>
       </c>
-      <c r="L22" t="s">
+      <c r="V22" t="s">
         <v>12</v>
       </c>
-      <c r="N22" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="O22" s="3">
+      <c r="X22" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y22" s="3">
         <v>9</v>
       </c>
-      <c r="P22" s="3"/>
+      <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8043,31 +9475,31 @@
       <c r="D23" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" t="s">
+      <c r="O23" s="3"/>
+      <c r="P23" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="R23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="S23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="J23" s="3">
+      <c r="T23" s="3">
         <v>448</v>
       </c>
-      <c r="L23" t="s">
+      <c r="V23" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="O23" s="3">
+      <c r="X23" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y23" s="3">
         <v>3308</v>
       </c>
-      <c r="P23" s="3"/>
+      <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8077,31 +9509,31 @@
       <c r="D24" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" t="s">
+      <c r="O24" s="3"/>
+      <c r="P24" t="s">
         <v>67</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="J24" s="3">
+      <c r="R24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="T24" s="3">
         <v>2</v>
       </c>
-      <c r="L24" t="s">
+      <c r="V24" t="s">
         <v>47</v>
       </c>
-      <c r="N24" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="O24" s="3">
+      <c r="X24" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y24" s="3">
         <v>1798</v>
       </c>
-      <c r="P24" s="3"/>
+      <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -8111,31 +9543,31 @@
       <c r="D25" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" t="s">
+      <c r="O25" s="3"/>
+      <c r="P25" t="s">
         <v>65</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="R25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="S25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J25" s="3">
+      <c r="T25" s="3">
         <v>3</v>
       </c>
-      <c r="L25" t="s">
-        <v>134</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="O25" s="3">
+      <c r="V25" t="s">
+        <v>133</v>
+      </c>
+      <c r="X25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y25" s="3">
         <v>44</v>
       </c>
-      <c r="P25" s="3"/>
+      <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -8145,31 +9577,31 @@
       <c r="D26" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" t="s">
+      <c r="O26" s="3"/>
+      <c r="P26" t="s">
         <v>55</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J26" s="3">
+      <c r="R26" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="T26" s="3">
         <v>30</v>
       </c>
-      <c r="L26" t="s">
+      <c r="V26" t="s">
         <v>9</v>
       </c>
-      <c r="N26" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="O26" s="3">
+      <c r="X26" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y26" s="3">
         <v>253</v>
       </c>
-      <c r="P26" s="3"/>
+      <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -8179,11 +9611,11 @@
       <c r="D27" t="s">
         <v>71</v>
       </c>
-      <c r="E27" t="s">
+      <c r="O27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -8193,11 +9625,11 @@
       <c r="D28" t="s">
         <v>69</v>
       </c>
-      <c r="E28" t="s">
+      <c r="O28" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -8207,20 +9639,20 @@
       <c r="D29" t="s">
         <v>69</v>
       </c>
-      <c r="F29" t="s">
+      <c r="P29" t="s">
         <v>47</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="J29" s="3">
+      <c r="R29" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="T29" s="3">
         <v>1606</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -8230,20 +9662,20 @@
       <c r="D30" t="s">
         <v>69</v>
       </c>
-      <c r="F30" t="s">
+      <c r="P30" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J30" s="3">
+      <c r="R30" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="T30" s="3">
         <v>219</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -8253,20 +9685,20 @@
       <c r="D31" t="s">
         <v>69</v>
       </c>
-      <c r="F31" t="s">
+      <c r="P31" t="s">
         <v>13</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="R31" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="S31" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J31" s="3">
+      <c r="T31" s="3">
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -8276,20 +9708,20 @@
       <c r="D32" t="s">
         <v>69</v>
       </c>
-      <c r="F32" t="s">
+      <c r="P32" t="s">
         <v>51</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="J32" s="3">
+      <c r="R32" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T32" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -8299,20 +9731,20 @@
       <c r="D33" t="s">
         <v>69</v>
       </c>
-      <c r="F33" t="s">
+      <c r="P33" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="R33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="S33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J33" s="3">
+      <c r="T33" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -8322,20 +9754,20 @@
       <c r="D34" t="s">
         <v>69</v>
       </c>
-      <c r="F34" t="s">
+      <c r="P34" t="s">
         <v>54</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="R34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="S34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="J34" s="3">
+      <c r="T34" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -8345,20 +9777,20 @@
       <c r="D35" t="s">
         <v>69</v>
       </c>
-      <c r="F35" t="s">
+      <c r="P35" t="s">
         <v>63</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="J35" s="3">
+      <c r="R35" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="S35" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="T35" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -8368,20 +9800,20 @@
       <c r="D36" t="s">
         <v>69</v>
       </c>
-      <c r="F36" t="s">
+      <c r="P36" t="s">
         <v>43</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="R36" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="S36" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="J36" s="3">
+      <c r="T36" s="3">
         <v>1644</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -8391,20 +9823,20 @@
       <c r="D37" t="s">
         <v>69</v>
       </c>
-      <c r="F37" t="s">
+      <c r="P37" t="s">
         <v>50</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="R37" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="S37" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="J37" s="3">
+      <c r="T37" s="3">
         <v>963</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -8414,20 +9846,20 @@
       <c r="D38" t="s">
         <v>69</v>
       </c>
-      <c r="F38" t="s">
+      <c r="P38" t="s">
         <v>2</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="R38" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="S38" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J38" s="3">
+      <c r="T38" s="3">
         <v>1178</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -8437,20 +9869,20 @@
       <c r="D39" t="s">
         <v>69</v>
       </c>
-      <c r="F39" t="s">
+      <c r="P39" t="s">
         <v>4</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="J39" s="3">
+      <c r="R39" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="T39" s="3">
         <v>569</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -8460,198 +9892,198 @@
       <c r="D40" t="s">
         <v>69</v>
       </c>
-      <c r="F40" t="s">
+      <c r="P40" t="s">
         <v>62</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="R40" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="S40" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="J40" s="3">
+      <c r="T40" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>38</v>
       </c>
-      <c r="F41" t="s">
+      <c r="P41" t="s">
         <v>48</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="R41" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="S41" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J41" s="3">
+      <c r="T41" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>39</v>
       </c>
-      <c r="F42" t="s">
+      <c r="P42" t="s">
         <v>26</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="R42" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="S42" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J42" s="3">
+      <c r="T42" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>40</v>
       </c>
-      <c r="F43" t="s">
+      <c r="P43" t="s">
         <v>3</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="J43" s="3">
+      <c r="R43" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="S43" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="T43" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
       </c>
-      <c r="F44" t="s">
+      <c r="P44" t="s">
         <v>61</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="R44" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="S44" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J44" s="3">
+      <c r="T44" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="F45" t="s">
+      <c r="P45" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="J45" s="3">
+      <c r="R45" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T45" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>43</v>
       </c>
-      <c r="E46" t="s">
+      <c r="O46" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>44</v>
       </c>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
     </row>
-    <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>45</v>
       </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
     </row>
-    <row r="49" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>21</v>
       </c>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
     </row>
-    <row r="50" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>46</v>
       </c>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
     </row>
-    <row r="51" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>47</v>
       </c>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
     </row>
-    <row r="52" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>48</v>
       </c>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
     </row>
-    <row r="53" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>49</v>
       </c>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -8659,7 +10091,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -8667,7 +10099,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -8675,7 +10107,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -8683,7 +10115,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -8691,7 +10123,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -8699,7 +10131,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -8707,7 +10139,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -8715,7 +10147,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -8723,7 +10155,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -8731,7 +10163,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Add DoubletFinder, FeaturePlot.1 and FeaturePlot.2
</commit_message>
<xml_diff>
--- a/doc/singler.colors.xlsx
+++ b/doc/singler.colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yah2014/Dropbox/Public/Olivier/Projects/scRNAseq-BladderCancer/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D94877A-86AA-3D43-B099-426550DC5220}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1563BC-E5EF-344C-A5E9-85D14998BF71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31480" yWindow="-6280" windowWidth="28760" windowHeight="16480" xr2:uid="{FD2BDCDE-9325-2D42-91C9-863AAE358120}"/>
+    <workbookView xWindow="8420" yWindow="460" windowWidth="21440" windowHeight="16480" xr2:uid="{FD2BDCDE-9325-2D42-91C9-863AAE358120}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -6722,8 +6722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1312DF4E-EAC9-0F41-8BFA-EBB9B641E9FE}">
   <dimension ref="A1:W91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>